<commit_message>
add account and type_list to Ready to deploy
</commit_message>
<xml_diff>
--- a/download_excel/kj.xlsx
+++ b/download_excel/kj.xlsx
@@ -206,7 +206,7 @@
     <t>2021-05-01-2021-05-31</t>
   </si>
   <si>
-    <t>2021-06-05</t>
+    <t>2021-06-18</t>
   </si>
   <si>
     <t>2</t>
@@ -2174,6 +2174,27 @@
     <t>2602</t>
   </si>
   <si>
+    <t>胖了哥甄选</t>
+  </si>
+  <si>
+    <t>admin2017666</t>
+  </si>
+  <si>
+    <t>//p26.douyinpic.com/img/tos-cn-avt-0015/0d62c0a0c09358f7ff449b0e39b2462a~c5_1080x1080.webp?from=2956013662</t>
+  </si>
+  <si>
+    <t>深圳市胖了哥甄选科技有限公司</t>
+  </si>
+  <si>
+    <t>42.43w</t>
+  </si>
+  <si>
+    <t>2513</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
     <t>中天潮购APP</t>
   </si>
   <si>
@@ -2187,27 +2208,6 @@
   </si>
   <si>
     <t>151.51w</t>
-  </si>
-  <si>
-    <t>2513</t>
-  </si>
-  <si>
-    <t>95</t>
-  </si>
-  <si>
-    <t>胖了哥甄选</t>
-  </si>
-  <si>
-    <t>admin2017666</t>
-  </si>
-  <si>
-    <t>//p26.douyinpic.com/img/tos-cn-avt-0015/0d62c0a0c09358f7ff449b0e39b2462a~c5_1080x1080.webp?from=2956013662</t>
-  </si>
-  <si>
-    <t>深圳市胖了哥甄选科技有限公司</t>
-  </si>
-  <si>
-    <t>42.43w</t>
   </si>
   <si>
     <t>96</t>
@@ -9101,10 +9101,10 @@
         <v>712</v>
       </c>
       <c r="H95" t="s" s="35">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="I95" t="s" s="35">
-        <v>425</v>
+        <v>312</v>
       </c>
       <c r="J95" t="s" s="35">
         <v>713</v>
@@ -9139,10 +9139,10 @@
         <v>719</v>
       </c>
       <c r="H96" t="s" s="35">
-        <v>295</v>
+        <v>309</v>
       </c>
       <c r="I96" t="s" s="35">
-        <v>312</v>
+        <v>425</v>
       </c>
       <c r="J96" t="s" s="35">
         <v>713</v>

</xml_diff>